<commit_message>
Update bill of materials with part numbers
</commit_message>
<xml_diff>
--- a/pcb_hardware/bill_of_materials.xlsx
+++ b/pcb_hardware/bill_of_materials.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="27540" windowHeight="15360" tabRatio="141"/>
+    <workbookView windowWidth="19260" windowHeight="8700" tabRatio="141"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102">
   <si>
     <t>Qty</t>
   </si>
@@ -29,6 +29,9 @@
     <t>Package</t>
   </si>
   <si>
+    <t>Manufactuer P/N</t>
+  </si>
+  <si>
     <t>Digikey P/N</t>
   </si>
   <si>
@@ -41,84 +44,120 @@
     <t>Description</t>
   </si>
   <si>
+    <t>Extended Price</t>
+  </si>
+  <si>
+    <t>(Total Qty at 120 boards)</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Min Qty</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>LED10MM</t>
+  </si>
+  <si>
+    <t>use 5mm  or alt</t>
+  </si>
+  <si>
+    <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10, D11, D12</t>
+  </si>
+  <si>
+    <t>LEDs</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>LED5MM</t>
+  </si>
+  <si>
+    <t>IR7393C</t>
+  </si>
+  <si>
+    <t>1080-1087-ND</t>
+  </si>
+  <si>
+    <t>D-IR1, D-IR2, D-IR3, D-IR4</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>TSOP382</t>
+  </si>
+  <si>
+    <t>TSOP38238</t>
+  </si>
+  <si>
+    <t>751-1227-ND</t>
+  </si>
+  <si>
+    <t>U1, U2</t>
+  </si>
+  <si>
+    <t>Vishay IR receiver module</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>RESISTOR0805-RES</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>ERJ-6GEYJ101V</t>
+  </si>
+  <si>
+    <t>P100ACT-ND</t>
+  </si>
+  <si>
+    <t>R13, R14, R15, R16, R18, R19, R20, R21</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>ERJ-6GEYJ103V</t>
+  </si>
+  <si>
+    <t>P10KACT-ND</t>
+  </si>
+  <si>
+    <t>R4, R27</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>JUMPER-2SMD-NO</t>
-  </si>
-  <si>
-    <t>SJ_2S-NO</t>
-  </si>
-  <si>
-    <t>JP2-RESET</t>
-  </si>
-  <si>
-    <t>Jumper</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>LED10MM</t>
-  </si>
-  <si>
-    <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10, D11, D12</t>
-  </si>
-  <si>
-    <t>LEDs</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>LED5MM</t>
-  </si>
-  <si>
-    <t>D-IR1, D-IR2, D-IR3, D-IR4</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>TSOP382</t>
-  </si>
-  <si>
-    <t>U1, U2</t>
-  </si>
-  <si>
-    <t>Vishay IR receiver module</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>RESISTOR0805-RES</t>
-  </si>
-  <si>
-    <t>0805</t>
-  </si>
-  <si>
-    <t>R13, R14, R15, R16, R18, R19, R20, R21</t>
-  </si>
-  <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>10K</t>
-  </si>
-  <si>
-    <t>R4, R27</t>
-  </si>
-  <si>
     <t>10nF</t>
   </si>
   <si>
     <t>CAP0805</t>
   </si>
   <si>
+    <t>CL21B103KBANNNC</t>
+  </si>
+  <si>
+    <t>1276-1015-2-ND</t>
+  </si>
+  <si>
     <t>C4</t>
   </si>
   <si>
@@ -128,12 +167,24 @@
     <t>10pF</t>
   </si>
   <si>
+    <t>CL21C100JBANNNC</t>
+  </si>
+  <si>
+    <t>1276-1109-1-ND</t>
+  </si>
+  <si>
     <t>C1, C3</t>
   </si>
   <si>
     <t>150</t>
   </si>
   <si>
+    <t>ERJ-6GEYJ151V</t>
+  </si>
+  <si>
+    <t>P150ACT-ND</t>
+  </si>
+  <si>
     <t>R23, R24, R25, R26</t>
   </si>
   <si>
@@ -146,6 +197,12 @@
     <t>HC49US</t>
   </si>
   <si>
+    <t>ATS16B</t>
+  </si>
+  <si>
+    <t>CTX1085-ND</t>
+  </si>
+  <si>
     <t>Y1</t>
   </si>
   <si>
@@ -158,12 +215,24 @@
     <t>1K</t>
   </si>
   <si>
+    <t>RC0805FR-071KL</t>
+  </si>
+  <si>
+    <t>311-1.00KCRCT-ND</t>
+  </si>
+  <si>
     <t>R1, R7, R8, R9, R10, R11, R30, R31, R32</t>
   </si>
   <si>
     <t>1uF</t>
   </si>
   <si>
+    <t>CC0805ZRY5V8BB105</t>
+  </si>
+  <si>
+    <t>311-1358-1-ND</t>
+  </si>
+  <si>
     <t>C2, C5</t>
   </si>
   <si>
@@ -173,19 +242,37 @@
     <t>2.2K</t>
   </si>
   <si>
+    <t>ERJ-6GEYJ222V</t>
+  </si>
+  <si>
+    <t>P2.2KACT-ND</t>
+  </si>
+  <si>
     <t>R5, R6, R12, R17, R22, R28, R29</t>
   </si>
   <si>
     <t>22</t>
   </si>
   <si>
+    <t>RPC0805JT22R0</t>
+  </si>
+  <si>
+    <t>RPC0805JT22R0CT-ND</t>
+  </si>
+  <si>
     <t>R2, R3</t>
   </si>
   <si>
     <t>ATMEGA32U4TQFP</t>
   </si>
   <si>
-    <t>SPARKFUN-DIGITALIC_TQFP44</t>
+    <t>TQFP44</t>
+  </si>
+  <si>
+    <t>ATMEGA32U4-AU</t>
+  </si>
+  <si>
+    <t>ATMEGA32U4-AU-ND</t>
   </si>
   <si>
     <t>IC1-AVR</t>
@@ -194,58 +281,46 @@
     <t>Atmel 44-pin 8-bit Microcontroller with 32KBytes of ISP Flash and USB Controller -----</t>
   </si>
   <si>
-    <t>AVR_SPI_PRG_6PTH</t>
-  </si>
-  <si>
-    <t>2X3</t>
-  </si>
-  <si>
-    <t>J1-ISP</t>
-  </si>
-  <si>
-    <t>AVR ISP 6 Pin</t>
-  </si>
-  <si>
-    <t>BINGHAMTON-EECE-TEXT</t>
-  </si>
-  <si>
-    <t>U$1</t>
-  </si>
-  <si>
-    <t>Binghamton University EECE Text Logo (Recomended!)</t>
-  </si>
-  <si>
-    <t>OSHW-LOGOM</t>
-  </si>
-  <si>
-    <t>OSHW-LOGO-M</t>
-  </si>
-  <si>
-    <t>LOGO1</t>
-  </si>
-  <si>
-    <t>Open Source Hardware Logo This logo indicates the piece of hardware it is found on incorporates a OSHW license and/or adheres to the definition of open source hardware found here: http://freedomdefined.org/OSHW</t>
-  </si>
-  <si>
     <t>PZT2222A</t>
   </si>
   <si>
     <t>SOT223</t>
   </si>
   <si>
+    <t>PZT2222AT1G</t>
+  </si>
+  <si>
+    <t>PZT2222AT1GOSTR-ND</t>
+  </si>
+  <si>
     <t>Q1, Q2, Q3, Q4, Q5, Q6, Q7</t>
   </si>
   <si>
+    <t>NPN Transistor</t>
+  </si>
+  <si>
     <t>USBSMD</t>
   </si>
   <si>
     <t>USB-MINIB</t>
   </si>
   <si>
+    <t>1734035-2</t>
+  </si>
+  <si>
+    <t>A31727CT-ND</t>
+  </si>
+  <si>
     <t>JP1</t>
   </si>
   <si>
     <t>USB Connectors</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -253,12 +328,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_(\$* #,##0_);_(\$* \(#,##0\);_(\$* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -273,12 +348,14 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Arial"/>
+      <b/>
+      <sz val="10"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="10"/>
       <name val="DejaVu Sans"/>
       <family val="2"/>
@@ -316,7 +393,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="1" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -331,22 +408,43 @@
     <xf numFmtId="41" fontId="1" fillId="0" borderId="1" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="5" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="5">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -663,18 +761,20 @@
         </a:custGeom>
         <a:gradFill rotWithShape="0">
           <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="BBD5F0"/>
+            </a:gs>
             <a:gs pos="100000">
               <a:srgbClr val="9CBEE0"/>
-            </a:gs>
-            <a:gs pos="0">
-              <a:srgbClr val="BBD5F0"/>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr val="739CC3"/>
+            <a:srgbClr val="739CC3">
+              <a:alpha val="100000"/>
+            </a:srgbClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="200000"/>
@@ -691,20 +791,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="G2" sqref="G2:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="4.19047619047619" style="2"/>
     <col min="2" max="3" width="21.8190476190476" style="2"/>
-    <col min="4" max="6" width="25.3714285714286" style="2"/>
-    <col min="7" max="7" width="41.5333333333333" style="2"/>
-    <col min="8" max="8" width="171.67619047619" style="2"/>
-    <col min="9" max="16384" width="9" style="2"/>
+    <col min="4" max="7" width="25.3714285714286" style="2"/>
+    <col min="8" max="8" width="41.5333333333333" style="2"/>
+    <col min="9" max="9" width="30.5714285714286" style="2" customWidth="1"/>
+    <col min="10" max="10" width="17.7142857142857" style="2" customWidth="1"/>
+    <col min="11" max="11" width="24.4285714285714" style="2" customWidth="1"/>
+    <col min="12" max="12" width="27.4285714285714" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1">
@@ -732,408 +835,727 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0.2864</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="5">
+        <f>G2*A2</f>
+        <v>3.4368</v>
+      </c>
+      <c r="K2" s="2">
+        <f>A2*120</f>
+        <v>1440</v>
+      </c>
+      <c r="L2" s="5">
+        <f>J2*120</f>
+        <v>412.416</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0.208</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="5">
+        <f t="shared" ref="J3:J17" si="0">G3*A3</f>
+        <v>0.832</v>
+      </c>
+      <c r="K3" s="2">
+        <f t="shared" ref="K3:K17" si="1">A3*120</f>
+        <v>480</v>
+      </c>
+      <c r="L3" s="5">
+        <f t="shared" ref="L3:L17" si="2">J3*120</f>
+        <v>99.84</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0.637</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>16</v>
+        <v>28</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="5">
+        <f>G4*A4</f>
+        <v>1.274</v>
+      </c>
+      <c r="K4" s="2">
+        <f>A4*120</f>
+        <v>240</v>
+      </c>
+      <c r="L4" s="5">
+        <f>J4*120</f>
+        <v>152.88</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0.00672</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>23</v>
+        <v>36</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="5">
+        <f>G5*A5</f>
+        <v>0.05376</v>
+      </c>
+      <c r="K5" s="2">
+        <f>A5*120</f>
+        <v>960</v>
+      </c>
+      <c r="L5" s="5">
+        <f>J5*120</f>
+        <v>6.4512</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>25</v>
+      <c r="B6" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0.00672</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>29</v>
+        <v>41</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="5">
+        <f>G6*A6</f>
+        <v>0.01344</v>
+      </c>
+      <c r="K6" s="2">
+        <f>A6*120</f>
+        <v>240</v>
+      </c>
+      <c r="L6" s="5">
+        <f>J6*120</f>
+        <v>1.6128</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0.00596</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" s="5">
+        <f>G7*A7</f>
+        <v>0.00596</v>
+      </c>
+      <c r="K7" s="2">
+        <f>A7*120</f>
+        <v>120</v>
+      </c>
+      <c r="L7" s="5">
+        <f>J7*120</f>
+        <v>0.7152</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="2" t="s">
-        <v>34</v>
+      <c r="E8" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0.0154</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>35</v>
+        <v>52</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" s="5">
+        <f>G8*A8</f>
+        <v>0.0308</v>
+      </c>
+      <c r="K8" s="2">
+        <f>A8*120</f>
+        <v>240</v>
+      </c>
+      <c r="L8" s="5">
+        <f>J8*120</f>
+        <v>3.696</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>36</v>
+        <v>19</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="2" t="s">
+      <c r="E9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.00672</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>35</v>
+      <c r="J9" s="5">
+        <f>G9*A9</f>
+        <v>0.02688</v>
+      </c>
+      <c r="K9" s="2">
+        <f>A9*120</f>
+        <v>480</v>
+      </c>
+      <c r="L9" s="5">
+        <f>J9*120</f>
+        <v>3.2256</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="2" t="s">
-        <v>39</v>
+        <v>58</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0.24</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>29</v>
+        <v>62</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" s="5">
+        <f>G10*A10</f>
+        <v>0.24</v>
+      </c>
+      <c r="K10" s="2">
+        <f>A10*120</f>
+        <v>120</v>
+      </c>
+      <c r="L10" s="5">
+        <f>J10*120</f>
+        <v>28.8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0.00381</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>44</v>
+        <v>68</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" s="5">
+        <f>G11*A11</f>
+        <v>0.03429</v>
+      </c>
+      <c r="K11" s="2">
+        <f>A11*120</f>
+        <v>1080</v>
+      </c>
+      <c r="L11" s="5">
+        <f>J11*120</f>
+        <v>4.1148</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="2" t="s">
-        <v>47</v>
+        <v>33</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0.01886</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>29</v>
+        <v>72</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="5">
+        <f>G12*A12</f>
+        <v>0.03772</v>
+      </c>
+      <c r="K12" s="2">
+        <f>A12*120</f>
+        <v>240</v>
+      </c>
+      <c r="L12" s="5">
+        <f>J12*120</f>
+        <v>4.5264</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="2" t="s">
-        <v>49</v>
+      <c r="E13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0.00448</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>35</v>
+        <v>77</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="5">
+        <f>G13*A13</f>
+        <v>0.03136</v>
+      </c>
+      <c r="K13" s="2">
+        <f>A13*120</f>
+        <v>840</v>
+      </c>
+      <c r="L13" s="5">
+        <f>J13*120</f>
+        <v>3.7632</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>51</v>
+        <v>24</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="2" t="s">
-        <v>52</v>
+        <v>33</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="8">
+        <v>0.06824</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>29</v>
+        <v>81</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J14" s="5">
+        <f>G14*A14</f>
+        <v>0.13648</v>
+      </c>
+      <c r="K14" s="2">
+        <f>A14*120</f>
+        <v>240</v>
+      </c>
+      <c r="L14" s="5">
+        <f>J14*120</f>
+        <v>16.3776</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>53</v>
+        <v>42</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="2" t="s">
-        <v>54</v>
+        <v>82</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="8">
+        <v>3.3684</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>29</v>
+        <v>86</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J15" s="5">
+        <f>G15*A15</f>
+        <v>3.3684</v>
+      </c>
+      <c r="K15" s="2">
+        <f>A15*120</f>
+        <v>120</v>
+      </c>
+      <c r="L15" s="5">
+        <f>J15*120</f>
+        <v>404.208</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>57</v>
+        <v>89</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" s="8">
+        <v>0.1032</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>58</v>
+        <v>92</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J16" s="5">
+        <f>G16*A16</f>
+        <v>0.7224</v>
+      </c>
+      <c r="K16" s="2">
+        <f>A16*120</f>
+        <v>840</v>
+      </c>
+      <c r="L16" s="5">
+        <f>J16*120</f>
+        <v>86.688</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>61</v>
+        <v>95</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G17" s="10">
+        <v>1.3698</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>62</v>
+        <v>98</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J17" s="5">
+        <f>G17*A17</f>
+        <v>1.3698</v>
+      </c>
+      <c r="K17" s="2">
+        <f>A17*120</f>
+        <v>120</v>
+      </c>
+      <c r="L17" s="5">
+        <f>J17*120</f>
+        <v>164.376</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="s">
-        <v>8</v>
+      <c r="A18" s="2">
+        <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>76</v>
+        <v>14</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="5">
+        <v>6</v>
+      </c>
+      <c r="J18" s="5">
+        <f>G18*A18</f>
+        <v>6</v>
+      </c>
+      <c r="K18" s="2">
+        <f>A18*120</f>
+        <v>120</v>
+      </c>
+      <c r="L18" s="5">
+        <f>J18*120</f>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="I22" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J22" s="5">
+        <f>SUM(J2:J21)</f>
+        <v>17.61409</v>
+      </c>
+      <c r="L22" s="5">
+        <f>SUM(L2:L21)</f>
+        <v>2113.6908</v>
       </c>
     </row>
   </sheetData>

</xml_diff>